<commit_message>
Update pipeline naming format and fix GUI version consistency
- 更新管道号格式为新标准："装置号和介质代码-管道号-管道尺寸-管道等级-保温等级"
- 修复GUI版本和核心逻辑版本不一致的问题
- 简化Excel输出格式为6列：管道号、管径、管道等级、保温等级、介质名称、相态
- 添加文本标准化处理，支持Unicode连字符清理
- 优化AutoCAD实体处理性能，增加进度显示
- 添加正则表达式自检和调试信息
- 重新打包exe文件，确保功能正常

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/test/code.xlsx
+++ b/test/code.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CAD2EXL\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3066B1F-103C-4B85-B216-78136E9AE6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20665814-D66E-4EB9-9617-4CC15CD67911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{78376A54-48F7-4543-A359-C37F4D4F1B4E}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
-  <si>
-    <t>BR</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>粗盐水</t>
   </si>
@@ -86,366 +83,379 @@
     <t>热水</t>
   </si>
   <si>
+    <t>生产上水</t>
+  </si>
+  <si>
+    <t>高压蒸气 (4MPaG)</t>
+  </si>
+  <si>
+    <t>高压蒸气冷凝液</t>
+  </si>
+  <si>
+    <t>中压蒸气 (1.5MPaG)</t>
+  </si>
+  <si>
+    <t>中压蒸气冷凝液</t>
+  </si>
+  <si>
+    <t>低压蒸气冷凝液</t>
+  </si>
+  <si>
+    <t>低低压蒸气冷凝液</t>
+  </si>
+  <si>
+    <t>液压油</t>
+  </si>
+  <si>
+    <t>低压氮气</t>
+  </si>
+  <si>
+    <t>中压氮气</t>
+  </si>
+  <si>
+    <t>高压氮气</t>
+  </si>
+  <si>
+    <t>泵密封水</t>
+  </si>
+  <si>
+    <t>放空气</t>
+  </si>
+  <si>
+    <t>安全阀放空</t>
+  </si>
+  <si>
+    <t>BRC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>过滤精盐水</t>
+  </si>
+  <si>
+    <t>CL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>36%氢氧化钠溶液</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>42%氢氧化钠溶液</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50%氢氧化钠溶液</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSP</t>
+  </si>
+  <si>
+    <t>DBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>淡盐水</t>
+  </si>
+  <si>
+    <t>DCBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>脱氯淡盐水</t>
+  </si>
+  <si>
+    <t>DSA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稀硫酸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>氢气冷凝液</t>
+  </si>
+  <si>
+    <t>FE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三氯化铁溶液</t>
+  </si>
+  <si>
+    <t>HAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稀盐酸</t>
+  </si>
+  <si>
+    <t>HA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31%高纯盐酸</t>
+  </si>
+  <si>
+    <t>HCL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>氯化氢气体</t>
+  </si>
+  <si>
+    <t>LCL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>液氯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>碳酸钠溶液</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>95~98%浓硫酸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>次氯酸钠溶液</t>
+  </si>
+  <si>
+    <t>SL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泥浆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工艺废水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>废气</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>循环上水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CWS</t>
+  </si>
+  <si>
+    <t>循环回水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CWR</t>
+  </si>
+  <si>
+    <t>冷冻上水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷冻回水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷冻盐水上水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSWS</t>
+  </si>
+  <si>
+    <t>冷冻盐水回水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSWR</t>
+  </si>
+  <si>
+    <t>生活水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>脱盐水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>液体氟利昂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FRL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>气体氟利昂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FRG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仪表空气</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工厂空气</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工艺冷凝液</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BRR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RWS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RWR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PTW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>PW</t>
-  </si>
-  <si>
-    <t>生产上水</t>
-  </si>
-  <si>
-    <t>高压蒸气 (4MPaG)</t>
-  </si>
-  <si>
-    <t>高压蒸气冷凝液</t>
-  </si>
-  <si>
-    <t>中压蒸气 (1.5MPaG)</t>
-  </si>
-  <si>
-    <t>中压蒸气冷凝液</t>
-  </si>
-  <si>
-    <t>低压蒸气 (0.4MPaG)</t>
-  </si>
-  <si>
-    <t>低压蒸气冷凝液</t>
-  </si>
-  <si>
-    <t>低低压蒸气</t>
-  </si>
-  <si>
-    <t>低低压蒸气冷凝液</t>
-  </si>
-  <si>
-    <t>液压油</t>
-  </si>
-  <si>
-    <t>低压氮气</t>
-  </si>
-  <si>
-    <t>中压氮气</t>
-  </si>
-  <si>
-    <t>高压氮气</t>
-  </si>
-  <si>
-    <t>泵密封水</t>
-  </si>
-  <si>
-    <t>放空气</t>
-  </si>
-  <si>
-    <t>安全阀放空</t>
-  </si>
-  <si>
-    <t>BRC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>过滤精盐水</t>
-  </si>
-  <si>
-    <t>CL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>36%氢氧化钠溶液</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>42%氢氧化钠溶液</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>50%氢氧化钠溶液</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSP</t>
-  </si>
-  <si>
-    <t>DBR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>淡盐水</t>
-  </si>
-  <si>
-    <t>DCBR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>脱氯淡盐水</t>
-  </si>
-  <si>
-    <t>DSA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>稀硫酸</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>氢气冷凝液</t>
-  </si>
-  <si>
-    <t>FE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>三氯化铁溶液</t>
-  </si>
-  <si>
-    <t>HAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>稀盐酸</t>
-  </si>
-  <si>
-    <t>HA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>31%高纯盐酸</t>
-  </si>
-  <si>
-    <t>HCL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>氯化氢气体</t>
-  </si>
-  <si>
-    <t>LCL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>液氯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>碳酸钠溶液</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PSUA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>95~98%浓硫酸</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>次氯酸钠溶液</t>
-  </si>
-  <si>
-    <t>SL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>泥浆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工艺废水</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>废气</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>循环上水</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CWS</t>
-  </si>
-  <si>
-    <t>循环回水</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CWR</t>
-  </si>
-  <si>
-    <t>CHWS</t>
-  </si>
-  <si>
-    <t>冷冻上水</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>冷冻回水</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CHWR</t>
-  </si>
-  <si>
-    <t>冷冻盐水上水</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSWS</t>
-  </si>
-  <si>
-    <t>冷冻盐水回水</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSWR</t>
-  </si>
-  <si>
-    <t>生活水</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>脱盐水</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>液体氟利昂</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FRL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>气体氟利昂</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FRG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>仪表空气</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LLS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LLC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工厂空气</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工艺冷凝液</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低压蒸气 (1.2MPaG)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低低压蒸气 (0.6MPaG)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WW</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -841,476 +851,484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A93B915-B23D-4364-B75D-4B0B58C8A254}">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
         <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
         <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
         <v>14</v>
-      </c>
-      <c r="B39" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B45" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A47" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A48" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B52" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A53" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B53" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A56" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A57" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A58" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B58" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.65">
+      <c r="A59" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>